<commit_message>
Mars project first part and user story updated
</commit_message>
<xml_diff>
--- a/MarsUserStory1.xlsx
+++ b/MarsUserStory1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My_IT_Prrojects\2_Project Mars\MyFirstMarsTask\MarsInternshipProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishal Desai\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F203A361-FB33-4C53-BEDC-98D7651A8BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08636500-9ACB-415F-96E6-8896DBBB5067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="171">
   <si>
     <t>Mars User Stories</t>
   </si>
@@ -194,15 +194,6 @@
     <t>1. Launch " http://localhost:5000/Home"</t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>User should be able to put relvent credentials</t>
-  </si>
-  <si>
-    <t>User should be able to check mark on term and condition buttton</t>
-  </si>
-  <si>
     <t>TC_ID_02</t>
   </si>
   <si>
@@ -212,11 +203,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>3. Enter all valid credentials
-(First Name : "Vishal" ; Last name : "Desai" Email -"desaivis@gmail.com"
-Password:" testmarssignup"; Confirm Password :" testmarslogin")</t>
-  </si>
-  <si>
     <t>3.Click "log in"</t>
   </si>
   <si>
@@ -238,21 +224,12 @@
     <t>User should be able to check mark on the button</t>
   </si>
   <si>
-    <t xml:space="preserve"> Verify If user is able to sign up  from home page</t>
-  </si>
-  <si>
     <t>5. Click Log out</t>
   </si>
   <si>
-    <t>Verify  that system recognize  users   log in credential when user have checked "remember me"  and user is log in agin with same browser</t>
-  </si>
-  <si>
     <t>6.Click "log in"</t>
   </si>
   <si>
-    <t>User should be able log in to the application with credentials already filled</t>
-  </si>
-  <si>
     <t>User should be able log out to the application</t>
   </si>
   <si>
@@ -268,24 +245,6 @@
     <t>5.Click on "edit button" on availability section &amp; click on "drop down" button to select "part time option"</t>
   </si>
   <si>
-    <t>6.Click on "edit button" on hours section &amp; click on "drop down button" to select "less than 30 hours" option</t>
-  </si>
-  <si>
-    <t>7.Click on "edit button" on hours section &amp; click on "earn target" to select ".between 500 and 100 per month" option</t>
-  </si>
-  <si>
-    <t>4. Check mark "Terms and conditions"</t>
-  </si>
-  <si>
-    <t>User should be able to click join button and window should pop up to put new join credential</t>
-  </si>
-  <si>
-    <t>5.Click on join button</t>
-  </si>
-  <si>
-    <t>User should be able to click join buttton and registered as new user</t>
-  </si>
-  <si>
     <t>Click on "sign in" button</t>
   </si>
   <si>
@@ -295,18 +254,6 @@
     <t xml:space="preserve">User should be able to enter user name and password credentials </t>
   </si>
   <si>
-    <t>2.Click "Join" button log in page</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> I want to register to the application portal by creating a usename and password so that application can remember me as a user and its credentials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a registered user, I want to log in without entering user name and password as credentials are already saved   as "remember me" </t>
-  </si>
-  <si>
-    <t>9.Click "Save" to save the profile</t>
-  </si>
-  <si>
     <t>2.Click "sign in"</t>
   </si>
   <si>
@@ -319,9 +266,6 @@
     <t>User should be abe to click on "edit button" and click on "drop down menu" to select "part time option"</t>
   </si>
   <si>
-    <t>User should be abe to click on "edit button" and click on "drop down menu" to select "less than 30 hours option option"</t>
-  </si>
-  <si>
     <t>User should be abe to click on "edit button" and click on drop down menu to select "between 500 and 1000 option"</t>
   </si>
   <si>
@@ -329,12 +273,6 @@
   </si>
   <si>
     <t>Verify if user able to select elements from profile   and "save" the preferences</t>
-  </si>
-  <si>
-    <t>As a registered user, I wan to select my preferences for "availability", "hours" and "earn target" from pull down menu and save them in my profile</t>
-  </si>
-  <si>
-    <t>As a registered user, I wan to write about my self in description tab to people know about my language and skills and save them in my profile</t>
   </si>
   <si>
     <t>User should be abe to click on description button</t>
@@ -452,15 +390,9 @@
     <t>Verify if user able to share skill from home page</t>
   </si>
   <si>
-    <t>As a registered user, I wan to add languages in my profile with limits &amp; also  cancel and delete it, if I don’t wan to add it.</t>
-  </si>
-  <si>
     <t>As a registered user, I want to add  skills in my profile &amp; also  cancel and delete it, if I don’t wan to add it.</t>
   </si>
   <si>
-    <t xml:space="preserve">As a registered user, I want to add  skills category to let people know about my service type, location type, available days and skill exchange </t>
-  </si>
-  <si>
     <t>TC_ID_09</t>
   </si>
   <si>
@@ -513,6 +445,133 @@
   </si>
   <si>
     <t>User_Story_11</t>
+  </si>
+  <si>
+    <t>Verify  that system recognize  users   log in credential when user have checked "remember me"  and user is log in with same browser</t>
+  </si>
+  <si>
+    <t>User should be abe to click on "edit button" and click on "drop down menu" to select "Full Time option"</t>
+  </si>
+  <si>
+    <t>6.Click on "edit button" on availability section &amp; click on "drop down" button to select "Full time option"</t>
+  </si>
+  <si>
+    <t>7.Click on "edit button" on hours section &amp; click on "drop down button" to select "less than 30 hours" option</t>
+  </si>
+  <si>
+    <t>8.Click on "edit button" on hours section &amp; click on "drop down button" to select " Morethan 30 hours" option</t>
+  </si>
+  <si>
+    <t>10.Click "Save" to save the profile</t>
+  </si>
+  <si>
+    <t>TC_ID_010</t>
+  </si>
+  <si>
+    <t>User_Story_12</t>
+  </si>
+  <si>
+    <t>As a registered user, I wan to select my preferences in profile section for "availability", "hours" and "earn target" from pull down menu and save them in my profile</t>
+  </si>
+  <si>
+    <t>User_Story_13</t>
+  </si>
+  <si>
+    <t>As a registered user, If I will put my username wrong , I want to be informed about my username credential is incorrect</t>
+  </si>
+  <si>
+    <t>As a registered user, If I will put my passowrd wrong , I want to be informed about my password credential is incorrect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a registered user, I want to log in without entering user name and password because credentials are already saved   as "remember me" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a registered user, I want to share  skills category to let people know about my service type, location type, available days and skill exchange </t>
+  </si>
+  <si>
+    <t>As a registered user, I want to add  skills category with mandatory fields and options fields , gives me postive testing with optional parameter</t>
+  </si>
+  <si>
+    <t>As a registered user, I want to add  skills category with mandatory fields and options fields , gives me nagative testing when put invalid credentials</t>
+  </si>
+  <si>
+    <t>As a registered user, I wan to add languages in my profile  &amp; also  cancel and delete it, if I don’t want to add it.</t>
+  </si>
+  <si>
+    <t>As a registered user, I wan to add languages max 4 languages in my profile &amp; also wants to check validate more than 4 languages are not accepted</t>
+  </si>
+  <si>
+    <t>Verify if username credential are incorrect, it gives error message for incorrect  username</t>
+  </si>
+  <si>
+    <t>3. User shouldbe be able to log in succesfully and go to the home page</t>
+  </si>
+  <si>
+    <t>3. Click on "log in" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to put username and  password credential, </t>
+  </si>
+  <si>
+    <t>User should be able to  get message when put incorrect username and correct password</t>
+  </si>
+  <si>
+    <t>Verify if password credential are incorrect, it gives error message for incorrect  password</t>
+  </si>
+  <si>
+    <t>2. Enter all correct username 
+(Email -"desaivis@gmail.com" and incorrect
+Password: "testmarslogin")</t>
+  </si>
+  <si>
+    <t>2. Enter all incorrect username 
+(Email -"kvdesai7@gmail.com" and correct
+Password: "testmarslogin")</t>
+  </si>
+  <si>
+    <t>User should be able to  get message when put correct username and incorrect password</t>
+  </si>
+  <si>
+    <t>User should be able log in succesfully to the application with credentials auto filled</t>
+  </si>
+  <si>
+    <t>9.Click on "edit button" on hours section &amp; click on "drop down button" to select " as needed" option</t>
+  </si>
+  <si>
+    <t>User should be abe to click on "edit button" and click on "drop down menu" to select "as needed" option"</t>
+  </si>
+  <si>
+    <t>User should be abe to click on "edit button" and click on "drop down menu" to select "More than than 30 hours option"</t>
+  </si>
+  <si>
+    <t>User should be abe to click on "edit button" and click on "drop down menu" to select "less than 30 hours option"</t>
+  </si>
+  <si>
+    <t>User should be abe to click on "edit button" and click on drop down menu to select "below 500 and option"</t>
+  </si>
+  <si>
+    <t>10.Click on "edit button" on hours section &amp; click on "earn target" to select ".below 500 per month" option</t>
+  </si>
+  <si>
+    <t>11.Click on "edit button" on hours section &amp; click on "earn target" to select ".between 500 and 1000 per month" option</t>
+  </si>
+  <si>
+    <t>12.Click on "edit button" on hours section &amp; click on "earn target" to select " more than 1000 per month" option</t>
+  </si>
+  <si>
+    <t>User should be abe to click on "edit button" and click on drop down menu to select " more than1000 option"</t>
+  </si>
+  <si>
+    <t>As a registered user, I wan to write about my self in description with max 100 words in tab to people know about my language and skills and save them in my profile</t>
+  </si>
+  <si>
+    <t>User_Story_14</t>
+  </si>
+  <si>
+    <t>As a registered user, I want error message when I put both username and password are correct but system givens error message for registation expired</t>
+  </si>
+  <si>
+    <t>As a registered user, I want error message when I Put both username and password are incorrect because they are not exist in system</t>
   </si>
 </sst>
 </file>
@@ -608,7 +667,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -733,19 +792,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right/>
@@ -883,9 +929,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -894,29 +937,23 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -956,28 +993,37 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1260,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,174 +1326,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
+      <c r="B1" s="37"/>
     </row>
     <row r="2" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="B2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
       <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
+      <c r="B3" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+    </row>
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+    </row>
+    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+    </row>
+    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
+      <c r="B7" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
+      <c r="B8" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
+      <c r="B9" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-    </row>
-    <row r="11" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="B11" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>151</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+    </row>
+    <row r="15" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -1467,19 +1559,35 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="15">
+    <mergeCell ref="B7:I7"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B4:I4"/>
     <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
     <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B15:I15"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B6:I6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1489,18 +1597,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7536C5B-B160-4E0B-8B2D-E9F3A5A05FE2}">
-  <dimension ref="A1:W68"/>
+  <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="78.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" customWidth="1"/>
+    <col min="4" max="4" width="60.28515625" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" style="24" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="24" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" style="24" customWidth="1"/>
@@ -1520,12 +1628,12 @@
         <v>15</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="26" t="s">
         <v>16</v>
       </c>
       <c r="H1" s="3"/>
@@ -1545,22 +1653,22 @@
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1578,20 +1686,18 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
     </row>
-    <row r="3" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
-      <c r="B3" s="47"/>
-      <c r="C3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>74</v>
+    <row r="3" spans="1:23" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>65</v>
       </c>
       <c r="E3" s="13"/>
-      <c r="F3" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="26"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1609,18 +1715,18 @@
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
     </row>
-    <row r="4" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+    <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1638,18 +1744,18 @@
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
     </row>
-    <row r="5" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>49</v>
+    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="42"/>
+      <c r="B5" s="46"/>
+      <c r="C5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1667,18 +1773,22 @@
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>76</v>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="E6" s="13"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1696,22 +1806,18 @@
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
     </row>
-    <row r="7" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="46" t="s">
-        <v>18</v>
-      </c>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="4" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1729,18 +1835,18 @@
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
     </row>
-    <row r="8" spans="1:23" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>78</v>
+    <row r="8" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>151</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1758,18 +1864,18 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
+    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1787,18 +1893,22 @@
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
     </row>
-    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="49"/>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="63" t="s">
+        <v>153</v>
+      </c>
       <c r="C10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>57</v>
+        <v>46</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1816,22 +1926,18 @@
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
     </row>
-    <row r="11" spans="1:23" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="46" t="s">
-        <v>63</v>
-      </c>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
+      <c r="B11" s="64"/>
       <c r="C11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>17</v>
+        <v>64</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>65</v>
       </c>
       <c r="E11" s="13"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1850,17 +1956,17 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="64"/>
       <c r="C12" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
+        <v>154</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1878,18 +1984,18 @@
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
     </row>
-    <row r="13" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="10" t="s">
-        <v>59</v>
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="45"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1907,18 +2013,22 @@
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
     </row>
-    <row r="14" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="47"/>
+    <row r="14" spans="1:23" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>130</v>
+      </c>
       <c r="C14" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E14" s="13"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1936,18 +2046,18 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
     </row>
-    <row r="15" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
+    <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1965,18 +2075,18 @@
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
     </row>
-    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="4" t="s">
-        <v>64</v>
+    <row r="16" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+        <v>56</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1994,22 +2104,18 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
     </row>
-    <row r="17" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="51" t="s">
-        <v>91</v>
-      </c>
+    <row r="17" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
+        <v>53</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -2027,18 +2133,18 @@
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
     </row>
-    <row r="18" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="52"/>
+    <row r="18" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
+        <v>57</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2056,18 +2162,18 @@
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
     </row>
-    <row r="19" spans="1:23" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
+    <row r="19" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="56"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2085,18 +2191,22 @@
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
     </row>
-    <row r="20" spans="1:23" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="52"/>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>73</v>
+      </c>
       <c r="C20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>86</v>
+        <v>46</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="E20" s="22"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2114,18 +2224,18 @@
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
     </row>
-    <row r="21" spans="1:23" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>87</v>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="41"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>65</v>
       </c>
       <c r="E21" s="22"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2143,18 +2253,18 @@
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
     </row>
-    <row r="22" spans="1:23" ht="72" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="52"/>
+    <row r="22" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="41"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>88</v>
+        <v>91</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="E22" s="22"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2172,18 +2282,18 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" spans="1:23" ht="72" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>89</v>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>69</v>
       </c>
       <c r="E23" s="22"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2201,513 +2311,748 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
     </row>
-    <row r="24" spans="1:23" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="4" t="s">
+    <row r="24" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="41"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="22"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+    </row>
+    <row r="25" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="22"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+    </row>
+    <row r="26" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="41"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="E26" s="22"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+    </row>
+    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" s="22"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+    </row>
+    <row r="28" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28" s="22"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+    </row>
+    <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="41"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29" s="22"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="41"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="22"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="41"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" s="22"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="42"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="22"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="21"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="41"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="21"/>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="41"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="21"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="41"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="21"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="41"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" s="21"/>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="42"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="21"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="21"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="41"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="21"/>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="41"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="21"/>
+    </row>
+    <row r="42" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="41"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="22"/>
-    </row>
-    <row r="25" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="51" t="s">
+      <c r="E42" s="21"/>
+    </row>
+    <row r="43" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="41"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="21"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="41"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" s="23"/>
+    </row>
+    <row r="45" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="A45" s="41"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="23"/>
+    </row>
+    <row r="46" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="41"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" s="23"/>
+    </row>
+    <row r="47" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="41"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" s="23"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="41"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="41"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="41"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D51" s="27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="41"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="41"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="39" x14ac:dyDescent="0.25">
+      <c r="A54" s="41"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="41"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="41"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D57" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="21"/>
-    </row>
-    <row r="26" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="4" t="s">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="53"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="53"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A60" s="53"/>
+      <c r="B60" s="55"/>
+      <c r="C60" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="53"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D61" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="21"/>
-    </row>
-    <row r="27" spans="1:23" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="21"/>
-    </row>
-    <row r="28" spans="1:23" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="21"/>
-    </row>
-    <row r="29" spans="1:23" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" s="21"/>
-    </row>
-    <row r="30" spans="1:23" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" s="21"/>
-    </row>
-    <row r="31" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="B31" s="51" t="s">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="53"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="39" x14ac:dyDescent="0.25">
+      <c r="A63" s="53"/>
+      <c r="B63" s="55"/>
+      <c r="C63" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="53"/>
+      <c r="B64" s="55"/>
+      <c r="C64" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D64" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="53"/>
+      <c r="B65" s="55"/>
+      <c r="C65" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="58"/>
+      <c r="B67" s="60"/>
+      <c r="C67" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="58"/>
+      <c r="B68" s="60"/>
+      <c r="C68" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A69" s="58"/>
+      <c r="B69" s="60"/>
+      <c r="C69" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="58"/>
+      <c r="B70" s="60"/>
+      <c r="C70" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="58"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="21"/>
-    </row>
-    <row r="32" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="21"/>
-    </row>
-    <row r="33" spans="1:5" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="E33" s="21"/>
-    </row>
-    <row r="34" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D34" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E34" s="21"/>
-    </row>
-    <row r="35" spans="1:5" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="21"/>
-    </row>
-    <row r="36" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="E36" s="23"/>
-    </row>
-    <row r="37" spans="1:5" ht="72" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" s="23"/>
-    </row>
-    <row r="38" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="23"/>
-    </row>
-    <row r="39" spans="1:5" ht="72" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="E39" s="23"/>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="B40" s="51" t="s">
+      <c r="D71" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="58"/>
+      <c r="B72" s="60"/>
+      <c r="C72" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A73" s="58"/>
+      <c r="B73" s="60"/>
+      <c r="C73" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
-      <c r="B41" s="52"/>
-      <c r="C41" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
-      <c r="B43" s="52"/>
-      <c r="C43" s="4" t="s">
+      <c r="D73" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D43" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
-      <c r="B44" s="52"/>
-      <c r="C44" s="4" t="s">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="58"/>
+      <c r="B74" s="60"/>
+      <c r="C74" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D74" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D44" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
-      <c r="B45" s="52"/>
-      <c r="C45" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D45" s="28" t="s">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="33"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="34"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="D76" s="27" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="52"/>
-      <c r="C46" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="52"/>
-      <c r="C47" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="44"/>
-      <c r="B48" s="52"/>
-      <c r="C48" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="D48" s="28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="B49" s="57" t="s">
-        <v>130</v>
-      </c>
-      <c r="C49" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="56"/>
-      <c r="B50" s="58"/>
-      <c r="C50" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="56"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="D51" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="56"/>
-      <c r="B52" s="58"/>
-      <c r="C52" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="D52" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="56"/>
-      <c r="B53" s="58"/>
-      <c r="C53" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D53" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="56"/>
-      <c r="B54" s="58"/>
-      <c r="C54" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="D54" s="28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="56"/>
-      <c r="B55" s="58"/>
-      <c r="C55" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D55" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="56"/>
-      <c r="B56" s="58"/>
-      <c r="C56" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="D56" s="28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="58.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="56"/>
-      <c r="B57" s="58"/>
-      <c r="C57" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="D57" s="28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="B58" s="62" t="s">
-        <v>130</v>
-      </c>
-      <c r="C58" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="61"/>
-      <c r="B59" s="63"/>
-      <c r="C59" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D59" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="61"/>
-      <c r="B60" s="63"/>
-      <c r="C60" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="D60" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="61"/>
-      <c r="B61" s="63"/>
-      <c r="C61" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="D61" s="28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="61"/>
-      <c r="B62" s="63"/>
-      <c r="C62" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="D62" s="28" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="61"/>
-      <c r="B63" s="63"/>
-      <c r="C63" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="D63" s="28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="61"/>
-      <c r="B64" s="63"/>
-      <c r="C64" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="D64" s="28" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="61"/>
-      <c r="B65" s="63"/>
-      <c r="C65" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D65" s="28" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="61"/>
-      <c r="B66" s="63"/>
-      <c r="C66" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="D66" s="28" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="34"/>
-      <c r="B67" s="36"/>
-      <c r="C67" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="D67" s="28" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="35"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="D68" s="28" t="s">
-        <v>150</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A49:A57"/>
-    <mergeCell ref="B49:B57"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="A58:A66"/>
-    <mergeCell ref="B58:B66"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="A31:A39"/>
-    <mergeCell ref="B31:B39"/>
-    <mergeCell ref="A40:A48"/>
-    <mergeCell ref="B40:B48"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B17:B24"/>
-    <mergeCell ref="A17:A24"/>
+  <mergeCells count="20">
+    <mergeCell ref="A57:A65"/>
+    <mergeCell ref="B57:B65"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A66:A74"/>
+    <mergeCell ref="B66:B74"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="A39:A47"/>
+    <mergeCell ref="B39:B47"/>
+    <mergeCell ref="A48:A56"/>
+    <mergeCell ref="B48:B56"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B20:B32"/>
+    <mergeCell ref="A20:A32"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2724,10 +3069,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="54" t="s">
+      <c r="A1" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -2739,8 +3084,8 @@
       <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="6" t="s">
         <v>21</v>
       </c>
@@ -2750,8 +3095,8 @@
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
@@ -2759,8 +3104,8 @@
       <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="6" t="s">
         <v>23</v>
       </c>
@@ -2768,8 +3113,8 @@
       <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
@@ -2777,45 +3122,45 @@
       <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="6"/>
       <c r="D6" s="12"/>
       <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="6"/>
       <c r="D7" s="12"/>
       <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="6"/>
       <c r="D8" s="12"/>
       <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="6"/>
       <c r="D9" s="12"/>
       <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="45"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="6"/>
       <c r="D10" s="12"/>
       <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="48" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -2827,8 +3172,8 @@
       <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="44"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
@@ -2838,8 +3183,8 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
@@ -2847,8 +3192,8 @@
       <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="8" t="s">
         <v>30</v>
       </c>
@@ -2856,8 +3201,8 @@
       <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="45"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="4" t="s">
         <v>31</v>
       </c>
@@ -2865,10 +3210,10 @@
       <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -2880,8 +3225,8 @@
       <c r="E16" s="21"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="4" t="s">
         <v>21</v>
       </c>
@@ -2891,8 +3236,8 @@
       <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
@@ -2900,8 +3245,8 @@
       <c r="E18" s="21"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
-      <c r="B19" s="45"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="4" t="s">
         <v>35</v>
       </c>
@@ -2909,10 +3254,10 @@
       <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="48" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -2924,8 +3269,8 @@
       <c r="E20" s="21"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="44"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="4" t="s">
         <v>21</v>
       </c>
@@ -2935,8 +3280,8 @@
       <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="44"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="5" t="s">
         <v>22</v>
       </c>
@@ -2944,8 +3289,8 @@
       <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="44"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="5" t="s">
         <v>39</v>
       </c>
@@ -2953,8 +3298,8 @@
       <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="42"/>
       <c r="C24" s="5" t="s">
         <v>40</v>
       </c>

</xml_diff>